<commit_message>
updated excel to put up to 49,999 values into graph
</commit_message>
<xml_diff>
--- a/BetterStayOnline/External/speedtestsTemplate.xlsx
+++ b/BetterStayOnline/External/speedtestsTemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joear\source\repos\BetterStayOnline\BetterStayOnline\External\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joear\Desktop\BSO\External\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6958845-4EA8-4EE5-9731-F45DA4DFB2CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28F8C373-ADA7-433D-99F2-0C7D7D337CD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="51480" yWindow="2610" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tests" sheetId="1" r:id="rId1"/>
@@ -215,19 +215,19 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>tests!$A$2:$A$157</c:f>
+              <c:f>tests!$A$2:$A$50000</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy\ h:mm</c:formatCode>
-                <c:ptCount val="156"/>
+                <c:ptCount val="49999"/>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>tests!$B$2:$B$157</c:f>
+              <c:f>tests!$B$2:$B$50000</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="156"/>
+                <c:ptCount val="49999"/>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -235,69 +235,6 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-AFC2-43A2-8496-723B5E37E751}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>tests!$C$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Upload</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>tests!$A$2:$A$157</c:f>
-              <c:numCache>
-                <c:formatCode>m/d/yyyy\ h:mm</c:formatCode>
-                <c:ptCount val="156"/>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>tests!$C$2:$C$157</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="156"/>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-AFC2-43A2-8496-723B5E37E751}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1419,7 +1356,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C164"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A49968" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>